<commit_message>
funções separadas e main organizada
</commit_message>
<xml_diff>
--- a/DT_OK.xlsx
+++ b/DT_OK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\excel-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DFE7AE-576F-4E3E-928C-A2FA19ECE976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BDD004-C39B-496B-B0F7-C9F895CFAE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="4" xr2:uid="{F4861128-A186-49E5-918A-C8C1B9913296}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{F4861128-A186-49E5-918A-C8C1B9913296}"/>
   </bookViews>
   <sheets>
     <sheet name="Visão Global" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -9142,7 +9142,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="665625" y="4029075"/>
+          <a:off x="665625" y="4038600"/>
           <a:ext cx="9030825" cy="2222500"/>
           <a:chOff x="667213" y="4101155"/>
           <a:chExt cx="9016537" cy="2185340"/>
@@ -9284,7 +9284,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4990080" y="4352925"/>
+          <a:off x="4990080" y="4362450"/>
           <a:ext cx="2191763" cy="435314"/>
           <a:chOff x="4990081" y="4044831"/>
           <a:chExt cx="1965757" cy="428974"/>
@@ -9610,7 +9610,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3638550" y="2305050"/>
+          <a:off x="3638550" y="2324100"/>
           <a:ext cx="6032499" cy="3552825"/>
           <a:chOff x="3638550" y="2667001"/>
           <a:chExt cx="6032499" cy="3253211"/>
@@ -10008,8 +10008,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1447800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>101780</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>87126</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -11460,7 +11460,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A294D240-2F63-4E90-AECB-C1D3D12B8871}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="71">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A294D240-2F63-4E90-AECB-C1D3D12B8871}" name="Tabela dinâmica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="71">
   <location ref="AB7:AH9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="72">
     <pivotField showAll="0"/>
@@ -11723,7 +11723,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A72B65D-3C72-4879-8602-8020DF072D6C}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A72B65D-3C72-4879-8602-8020DF072D6C}" name="Tabela dinâmica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="U42:U52" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="72">
     <pivotField showAll="0"/>
@@ -13613,7 +13613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:24">
+    <row r="16" spans="2:24" ht="15.75">
       <c r="D16" s="146"/>
       <c r="E16" s="148" t="s">
         <v>188</v>
@@ -14124,7 +14124,7 @@
       <c r="C13" s="17"/>
       <c r="D13" s="10">
         <f>SUM(Dados[IR &amp; IOF | Mês Atual])</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="113" t="s">
@@ -14190,7 +14190,7 @@
       <c r="C15" s="17"/>
       <c r="D15" s="116">
         <f>SUM(Dados[Saldo Líquido | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="83" t="str">
@@ -14312,7 +14312,7 @@
       <c r="O19" s="118"/>
       <c r="P19" s="120"/>
     </row>
-    <row r="20" spans="2:16">
+    <row r="20" spans="2:16" ht="15.75">
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="2:16" ht="15.75">
@@ -14380,7 +14380,7 @@
     <col min="34" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34">
+    <row r="1" spans="2:34" ht="15.75">
       <c r="B1" s="196" t="s">
         <v>164</v>
       </c>
@@ -14389,7 +14389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:34">
+    <row r="2" spans="2:34" ht="15.75">
       <c r="B2" s="196" t="s">
         <v>164</v>
       </c>
@@ -17163,7 +17163,9 @@
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC6" s="56"/>
+      <c r="AC6" s="56">
+        <v>100</v>
+      </c>
       <c r="AE6" s="56"/>
       <c r="AF6" s="56"/>
       <c r="AI6" s="56"/>
@@ -17193,7 +17195,7 @@
       </c>
       <c r="AT6" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AU6" s="180">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
@@ -17201,7 +17203,7 @@
       </c>
       <c r="AV6" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AW6" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
@@ -18991,7 +18993,7 @@
       <c r="BR16" s="50"/>
       <c r="BS16" s="50"/>
     </row>
-    <row r="17" spans="2:71" ht="11.25" hidden="1">
+    <row r="17" spans="2:71" ht="11.25">
       <c r="B17" s="157" t="str">
         <f>IF(Dados[[#This Row],[Tipo do Ativo]]="","",Dados[[#This Row],[Tipo do Ativo]]&amp;" ")&amp;IF(Dados[[#This Row],[Emissor]]="","",Dados[[#This Row],[Emissor]])&amp;IF(Dados[[#This Row],[Vencimento]]="",""," "&amp;TEXT(Dados[[#This Row],[Vencimento]],"mm/aa"))&amp;IF(Dados[[#This Row],[Remuneração]]="",""," "&amp;TEXT(Dados[[#This Row],[Remuneração]],"##,##%"))&amp;IF(Dados[[#This Row],[Complemento]]="",""," "&amp;Dados[[#This Row],[Complemento]])</f>
         <v>Previdencia 1</v>
@@ -19163,7 +19165,7 @@
       <c r="BR17" s="50"/>
       <c r="BS17" s="50"/>
     </row>
-    <row r="18" spans="2:71" ht="11.25" hidden="1">
+    <row r="18" spans="2:71" ht="11.25">
       <c r="B18" s="157" t="str">
         <f>IF(Dados[[#This Row],[Tipo do Ativo]]="","",Dados[[#This Row],[Tipo do Ativo]]&amp;" ")&amp;IF(Dados[[#This Row],[Emissor]]="","",Dados[[#This Row],[Emissor]])&amp;IF(Dados[[#This Row],[Vencimento]]="",""," "&amp;TEXT(Dados[[#This Row],[Vencimento]],"mm/aa"))&amp;IF(Dados[[#This Row],[Remuneração]]="",""," "&amp;TEXT(Dados[[#This Row],[Remuneração]],"##,##%"))&amp;IF(Dados[[#This Row],[Complemento]]="",""," "&amp;Dados[[#This Row],[Complemento]])</f>
         <v>Previdencia 2</v>
@@ -19335,7 +19337,7 @@
       <c r="BR18" s="50"/>
       <c r="BS18" s="50"/>
     </row>
-    <row r="19" spans="2:71" ht="11.25" hidden="1">
+    <row r="19" spans="2:71" ht="11.25">
       <c r="B19" s="157" t="str">
         <f>IF(Dados[[#This Row],[Tipo do Ativo]]="","",Dados[[#This Row],[Tipo do Ativo]]&amp;" ")&amp;IF(Dados[[#This Row],[Emissor]]="","",Dados[[#This Row],[Emissor]])&amp;IF(Dados[[#This Row],[Vencimento]]="",""," "&amp;TEXT(Dados[[#This Row],[Vencimento]],"mm/aa"))&amp;IF(Dados[[#This Row],[Remuneração]]="",""," "&amp;TEXT(Dados[[#This Row],[Remuneração]],"##,##%"))&amp;IF(Dados[[#This Row],[Complemento]]="",""," "&amp;Dados[[#This Row],[Complemento]])</f>
         <v>Prev. BTG Cred Corp II FI MULT CP</v>
@@ -19500,7 +19502,7 @@
       <c r="BR19" s="50"/>
       <c r="BS19" s="50"/>
     </row>
-    <row r="20" spans="2:71" ht="11.25" hidden="1">
+    <row r="20" spans="2:71" ht="11.25">
       <c r="B20" s="157" t="str">
         <f>IF(Dados[[#This Row],[Tipo do Ativo]]="","",Dados[[#This Row],[Tipo do Ativo]]&amp;" ")&amp;IF(Dados[[#This Row],[Emissor]]="","",Dados[[#This Row],[Emissor]])&amp;IF(Dados[[#This Row],[Vencimento]]="",""," "&amp;TEXT(Dados[[#This Row],[Vencimento]],"mm/aa"))&amp;IF(Dados[[#This Row],[Remuneração]]="",""," "&amp;TEXT(Dados[[#This Row],[Remuneração]],"##,##%"))&amp;IF(Dados[[#This Row],[Complemento]]="",""," "&amp;Dados[[#This Row],[Complemento]])</f>
         <v>Prev. Éxes FIE FC FI Mult Cred Priv</v>

</xml_diff>

<commit_message>
filtragem de entrada de dados no input das celulas
</commit_message>
<xml_diff>
--- a/DT_OK.xlsx
+++ b/DT_OK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="EstaPastaDeTrabalho" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\excel-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BDD004-C39B-496B-B0F7-C9F895CFAE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B54AA11-AAC2-479D-A917-E78980FA7668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{F4861128-A186-49E5-918A-C8C1B9913296}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{F4861128-A186-49E5-918A-C8C1B9913296}"/>
   </bookViews>
   <sheets>
     <sheet name="Visão Global" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -783,13 +783,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="6">
+  <numFmts count="8">
+    <numFmt numFmtId="7" formatCode="&quot;R$&quot;\ #,##0.00;\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-416]mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-[$USD]\ * #,##0.0000_-;\-[$USD]\ * #,##0.0000_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;R$&quot;\ * #.##000_-;\-&quot;R$&quot;\ * #.##000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -1351,7 +1353,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="242">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2012,6 +2014,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4312,7 +4326,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.81818181818181823</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4368,7 +4382,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>9.0909090909090912E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4424,7 +4438,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>9.0909090909090912E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5550,28 +5564,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.45454545454545459</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.54545454545454553</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.90909090909090917</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9142,7 +9156,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="665625" y="4038600"/>
+          <a:off x="665625" y="4029075"/>
           <a:ext cx="9030825" cy="2222500"/>
           <a:chOff x="667213" y="4101155"/>
           <a:chExt cx="9016537" cy="2185340"/>
@@ -9284,7 +9298,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4990080" y="4362450"/>
+          <a:off x="4990080" y="4352925"/>
           <a:ext cx="2191763" cy="435314"/>
           <a:chOff x="4990081" y="4044831"/>
           <a:chExt cx="1965757" cy="428974"/>
@@ -9610,7 +9624,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3638550" y="2324100"/>
+          <a:off x="3638550" y="2305050"/>
           <a:ext cx="6032499" cy="3552825"/>
           <a:chOff x="3638550" y="2667001"/>
           <a:chExt cx="6032499" cy="3253211"/>
@@ -9930,7 +9944,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1438274</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>123920</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -9940,7 +9954,7 @@
             <xdr:cNvPr id="4" name="Custódia">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10002,14 +10016,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>123920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1447800</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>87126</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>72472</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -10018,7 +10032,7 @@
             <xdr:cNvPr id="5" name="Nomenclatura Classe">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11460,7 +11474,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A294D240-2F63-4E90-AECB-C1D3D12B8871}" name="Tabela dinâmica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="71">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A294D240-2F63-4E90-AECB-C1D3D12B8871}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="71">
   <location ref="AB7:AH9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="72">
     <pivotField showAll="0"/>
@@ -11723,7 +11737,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A72B65D-3C72-4879-8602-8020DF072D6C}" name="Tabela dinâmica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A72B65D-3C72-4879-8602-8020DF072D6C}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="U42:U52" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="72">
     <pivotField showAll="0"/>
@@ -11908,19 +11922,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D4CD5E1-FC1C-4A55-B0A5-1B57589F6FBC}" name="Dados" displayName="Dados" ref="B5:BL20" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
-  <autoFilter ref="B5:BL20" xr:uid="{6D4CD5E1-FC1C-4A55-B0A5-1B57589F6FBC}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="BTG"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="18">
-      <filters>
-        <filter val="Renda Fixa - Inflação"/>
-        <filter val="Renda Fixa - Prefixado"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B5:BL20" xr:uid="{6D4CD5E1-FC1C-4A55-B0A5-1B57589F6FBC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:BL18">
     <sortCondition ref="B5:B18"/>
   </sortState>
@@ -13426,7 +13428,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="8">
         <f>SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="H5" s="9">
         <v>1</v>
@@ -13450,11 +13452,11 @@
       <c r="F6" s="17"/>
       <c r="G6" s="11">
         <f>SUMIF(Dados[Custódia],B6,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="150" t="str">
+        <v>900</v>
+      </c>
+      <c r="H6" s="150">
         <f t="shared" ref="H6" si="1">IFERROR(G6/$G$5,"ERRO")</f>
-        <v>ERRO</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="I6" s="6"/>
     </row>
@@ -13474,11 +13476,11 @@
       <c r="F7" s="17"/>
       <c r="G7" s="10">
         <f>SUMIF(Dados[Custódia],B7,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="13" t="str">
+        <v>100</v>
+      </c>
+      <c r="H7" s="13">
         <f t="shared" ref="H7:H8" si="3">IFERROR(G7/$G$5,"ERRO")</f>
-        <v>ERRO</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="I7" s="6"/>
     </row>
@@ -13498,11 +13500,11 @@
       <c r="F8" s="17"/>
       <c r="G8" s="11">
         <f>SUMIF(Dados[Custódia],B8,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="150" t="str">
+        <v>100</v>
+      </c>
+      <c r="H8" s="150">
         <f t="shared" si="3"/>
-        <v>ERRO</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="I8" s="6"/>
     </row>
@@ -13552,7 +13554,7 @@
       <c r="F11" s="140"/>
       <c r="G11" s="138">
         <f>G5</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="H11" s="139" t="e">
         <f>_xlfn.XLOOKUP(G3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Performance Carteira])</f>
@@ -13610,10 +13612,10 @@
       </c>
       <c r="U15" s="127">
         <f>SUM(U18:U22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:24" ht="15.75">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24">
       <c r="D16" s="146"/>
       <c r="E16" s="148" t="s">
         <v>188</v>
@@ -13665,15 +13667,15 @@
       </c>
       <c r="U18" s="29">
         <f>SUMIF(Dados[Custódia],S18,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="W18" s="31">
         <f>T18/$T$15</f>
         <v>1</v>
       </c>
-      <c r="X18" s="31" t="e">
+      <c r="X18" s="31">
         <f>U18/$U$15</f>
-        <v>#DIV/0!</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="19" spans="4:24">
@@ -13690,15 +13692,15 @@
       </c>
       <c r="U19" s="152">
         <f>SUMIF(Dados[Custódia],S19,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W19" s="153">
         <f>T19/$T$15</f>
         <v>0</v>
       </c>
-      <c r="X19" s="153" t="e">
+      <c r="X19" s="153">
         <f>U19/$U$15</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="20" spans="4:24">
@@ -13715,15 +13717,15 @@
       </c>
       <c r="U20" s="29">
         <f>SUMIF(Dados[Custódia],S20,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W20" s="31">
         <f>T20/$T$15</f>
         <v>0</v>
       </c>
-      <c r="X20" s="31" t="e">
+      <c r="X20" s="31">
         <f>U20/$U$15</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="21" spans="4:24">
@@ -13744,9 +13746,9 @@
         <f>T21/$T$15</f>
         <v>0</v>
       </c>
-      <c r="X21" s="153" t="e">
+      <c r="X21" s="153">
         <f>U21/$U$15</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="4:24">
@@ -13766,9 +13768,9 @@
         <f>T22/$T$15</f>
         <v>0</v>
       </c>
-      <c r="X22" s="31" t="e">
+      <c r="X22" s="31">
         <f>U22/$U$15</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="4:24">
@@ -13860,7 +13862,7 @@
     <row r="2" spans="2:16">
       <c r="B2" s="201">
         <f>SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="201" t="e">
@@ -14084,7 +14086,7 @@
       <c r="C12" s="15"/>
       <c r="D12" s="112">
         <f>SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="108" t="s">
@@ -14124,7 +14126,7 @@
       <c r="C13" s="17"/>
       <c r="D13" s="10">
         <f>SUM(Dados[IR &amp; IOF | Mês Atual])</f>
-        <v>-100</v>
+        <v>-1600</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="113" t="s">
@@ -14190,7 +14192,7 @@
       <c r="C15" s="17"/>
       <c r="D15" s="116">
         <f>SUM(Dados[Saldo Líquido | Mês Atual])</f>
-        <v>100</v>
+        <v>2700</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="83" t="str">
@@ -14312,7 +14314,7 @@
       <c r="O19" s="118"/>
       <c r="P19" s="120"/>
     </row>
-    <row r="20" spans="2:16" ht="15.75">
+    <row r="20" spans="2:16">
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="2:16" ht="15.75">
@@ -14380,22 +14382,22 @@
     <col min="34" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="15.75">
+    <row r="1" spans="2:34">
       <c r="B1" s="196" t="s">
         <v>164</v>
       </c>
       <c r="C1" s="197">
         <f>SUM(Dados[Saldo Bruto | Mês Atual])*2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="2:34" ht="15.75">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="2" spans="2:34">
       <c r="B2" s="196" t="s">
         <v>164</v>
       </c>
       <c r="C2" s="197">
         <f>SUM(C7:C30)</f>
-        <v>0</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="4" spans="2:34" ht="15.75">
@@ -14432,7 +14434,7 @@
       </c>
       <c r="Y5" s="127">
         <f>SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="6" spans="2:34">
@@ -14468,9 +14470,9 @@
         <v>51</v>
       </c>
       <c r="C7" s="100"/>
-      <c r="D7" s="77" t="str">
+      <c r="D7" s="77">
         <f>IFERROR(SUMIF(Dados[Classe],B7,Dados[Saldo Bruto | Mês Atual])/SUM(Dados[Saldo Bruto | Mês Atual]),"ERRO")</f>
-        <v>ERRO</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="F7" s="89" t="str" cm="1">
         <f t="array" ref="F7:F9">_xlfn._xlws.SORT(_xlfn.UNIQUE(Dados[Custódia]))</f>
@@ -14488,15 +14490,15 @@
       <c r="J7" s="94"/>
       <c r="K7" s="69">
         <f>SUMIF(Dados[Custódia],F7,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="L7" s="90">
         <f>SUMIF(Dados[Custódia],F7,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="M7" s="72" t="e">
+      <c r="M7" s="72">
         <f>K7/$K$10</f>
-        <v>#DIV/0!</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="S7" s="159" t="s">
         <v>178</v>
@@ -14527,11 +14529,11 @@
       </c>
       <c r="C8" s="210">
         <f>SUMIF(Dados[Subclasse],B8,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="150" t="e">
+        <v>300</v>
+      </c>
+      <c r="D8" s="150">
         <f>C8/$C$16</f>
-        <v>#DIV/0!</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="F8" s="1" t="str">
         <v>Safra</v>
@@ -14548,15 +14550,15 @@
       <c r="J8" s="94"/>
       <c r="K8" s="10">
         <f>SUMIF(Dados[Custódia],F8,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L8" s="189">
         <f>SUMIF(Dados[Custódia],F8,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="M8" s="190" t="e">
+      <c r="M8" s="190">
         <f>K8/$K$10</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="S8" t="str" cm="1">
         <f t="array" ref="S8:S11">_xlfn.UNIQUE(Dados[Classe])</f>
@@ -14571,15 +14573,15 @@
       </c>
       <c r="X8" s="161">
         <f>SUMIF(Dados[Liquidez],W8,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="Y8" s="162" t="str">
+        <v>400</v>
+      </c>
+      <c r="Y8" s="162">
         <f>IFERROR(X8/$Y$5,"ERRO")</f>
-        <v>ERRO</v>
-      </c>
-      <c r="Z8" s="162" t="str">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="Z8" s="162">
         <f>Y8</f>
-        <v>ERRO</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="AC8" t="s">
         <v>41</v>
@@ -14605,9 +14607,9 @@
         <v>52</v>
       </c>
       <c r="C9" s="100"/>
-      <c r="D9" s="77" t="str">
+      <c r="D9" s="77">
         <f>IFERROR(SUMIF(Dados[Classe],B9,Dados[Saldo Bruto | Mês Atual])/SUM(Dados[Saldo Bruto | Mês Atual]),"ERRO")</f>
-        <v>ERRO</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="F9" s="89" t="str">
         <v>Santander</v>
@@ -14624,15 +14626,15 @@
       <c r="J9" s="94"/>
       <c r="K9" s="69">
         <f>SUMIF(Dados[Custódia],F9,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L9" s="90">
         <f>SUMIF(Dados[Custódia],F9,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="M9" s="72" t="e">
+      <c r="M9" s="72">
         <f>K9/$K$10</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="S9" t="str">
         <v>Renda Fixa</v>
@@ -14647,13 +14649,13 @@
         <f>SUMIF(Dados[Liquidez],W9,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y9" s="164" t="str">
+      <c r="Y9" s="164">
         <f>IFERROR(X9/$Y$5,"ERRO")</f>
-        <v>ERRO</v>
-      </c>
-      <c r="Z9" s="164" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="164">
         <f>IFERROR(Y9+Z8,"ERRO")</f>
-        <v>ERRO</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="AB9" t="s">
         <v>119</v>
@@ -14684,11 +14686,11 @@
       </c>
       <c r="C10" s="14">
         <f>SUMIF(Dados[Subclasse],B10,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="13" t="e">
+        <v>200</v>
+      </c>
+      <c r="D10" s="13">
         <f>C10/$C$16</f>
-        <v>#DIV/0!</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="F10" s="95" t="s">
         <v>104</v>
@@ -14704,7 +14706,7 @@
       <c r="J10" s="98"/>
       <c r="K10" s="97">
         <f>SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="L10" s="97">
         <f>SUM(Dados[Movimentaçao | Mês Atual])</f>
@@ -14726,13 +14728,13 @@
         <f>SUMIF(Dados[Liquidez],W10,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y10" s="162" t="str">
+      <c r="Y10" s="162">
         <f t="shared" ref="Y10:Y16" si="0">IFERROR(X10/$Y$5,"ERRO")</f>
-        <v>ERRO</v>
-      </c>
-      <c r="Z10" s="162" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="162">
         <f t="shared" ref="Z10:Z14" si="1">IFERROR(Y10+Z9,"ERRO")</f>
-        <v>ERRO</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="11" spans="2:34">
@@ -14741,11 +14743,11 @@
       </c>
       <c r="C11" s="101">
         <f>SUMIF(Dados[Subclasse],B11,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="71" t="e">
+        <v>500</v>
+      </c>
+      <c r="D11" s="71">
         <f>C11/$C$16</f>
-        <v>#DIV/0!</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="S11" t="str">
         <v>Previdência</v>
@@ -14758,15 +14760,15 @@
       </c>
       <c r="X11" s="163">
         <f>SUMIF(Dados[Liquidez],W11,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="Y11" s="164" t="str">
+        <v>100</v>
+      </c>
+      <c r="Y11" s="164">
         <f t="shared" si="0"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z11" s="164" t="str">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="Z11" s="164">
         <f t="shared" si="1"/>
-        <v>ERRO</v>
+        <v>0.45454545454545459</v>
       </c>
     </row>
     <row r="12" spans="2:34">
@@ -14774,9 +14776,9 @@
         <v>183</v>
       </c>
       <c r="C12" s="100"/>
-      <c r="D12" s="77" t="str">
+      <c r="D12" s="77">
         <f>IFERROR(SUMIF(Dados[Classe],B12,Dados[Saldo Bruto | Mês Atual])/SUM(Dados[Saldo Bruto | Mês Atual]),"ERRO")</f>
-        <v>ERRO</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="F12" s="99" t="s">
         <v>115</v>
@@ -14793,15 +14795,15 @@
       </c>
       <c r="X12" s="161">
         <f>SUMIF(Dados[Liquidez],W12,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="Y12" s="162" t="str">
+        <v>100</v>
+      </c>
+      <c r="Y12" s="162">
         <f t="shared" si="0"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z12" s="162" t="str">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="Z12" s="162">
         <f t="shared" si="1"/>
-        <v>ERRO</v>
+        <v>0.54545454545454553</v>
       </c>
     </row>
     <row r="13" spans="2:34">
@@ -14811,11 +14813,11 @@
       </c>
       <c r="C13" s="14">
         <f>SUMIF(Dados[Subclasse],B13,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="13" t="e">
+        <v>100</v>
+      </c>
+      <c r="D13" s="13">
         <f>C13/$C$16</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="U13" s="158" t="str">
         <v>D+0</v>
@@ -14825,15 +14827,15 @@
       </c>
       <c r="X13" s="163">
         <f>SUMIF(Dados[Liquidez],W13,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="Y13" s="164" t="str">
+        <v>400</v>
+      </c>
+      <c r="Y13" s="164">
         <f t="shared" si="0"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z13" s="164" t="str">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="Z13" s="164">
         <f t="shared" si="1"/>
-        <v>ERRO</v>
+        <v>0.90909090909090917</v>
       </c>
     </row>
     <row r="14" spans="2:34">
@@ -14841,9 +14843,9 @@
         <v>57</v>
       </c>
       <c r="C14" s="100"/>
-      <c r="D14" s="77" t="str">
+      <c r="D14" s="77">
         <f>IFERROR(SUMIF(Dados[Classe],B14,Dados[Saldo Bruto | Mês Atual])/SUM(Dados[Saldo Bruto | Mês Atual]),"ERRO")</f>
-        <v>ERRO</v>
+        <v>0</v>
       </c>
       <c r="U14" s="158" t="str">
         <v>D+3</v>
@@ -14853,15 +14855,15 @@
       </c>
       <c r="X14" s="161">
         <f>SUMIF(Dados[Liquidez],W14,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
-      </c>
-      <c r="Y14" s="162" t="str">
+        <v>100</v>
+      </c>
+      <c r="Y14" s="162">
         <f t="shared" si="0"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z14" s="162" t="str">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="Z14" s="162">
         <f t="shared" si="1"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:34">
@@ -14873,9 +14875,9 @@
         <f>SUMIF(Dados[Subclasse],B15,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="D15" s="71" t="e">
+      <c r="D15" s="71">
         <f>C15/$C$16</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="U15" s="158" t="str">
         <v>D+7</v>
@@ -14887,13 +14889,13 @@
         <f>SUMIF(Dados[Liquidez],W15,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y15" s="164" t="str">
+      <c r="Y15" s="164">
         <f t="shared" si="0"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z15" s="164" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="164">
         <f t="shared" ref="Z15" si="2">IFERROR(Y15+Z14,"ERRO")</f>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:34">
@@ -14902,7 +14904,7 @@
       </c>
       <c r="C16" s="85">
         <f>SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="D16" s="86">
         <v>1</v>
@@ -14911,13 +14913,13 @@
         <f>SUMIF(Dados[Liquidez],W16,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y16" s="162" t="str">
+      <c r="Y16" s="162">
         <f t="shared" si="0"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z16" s="162" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="162">
         <f>IFERROR(Y16+Z15,"ERRO")</f>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="23:26">
@@ -14926,13 +14928,13 @@
         <f>SUMIF(Dados[Liquidez],W17,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y17" s="164" t="str">
+      <c r="Y17" s="164">
         <f t="shared" ref="Y17:Y23" si="3">IFERROR(X17/$Y$5,"ERRO")</f>
-        <v>ERRO</v>
-      </c>
-      <c r="Z17" s="164" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="164">
         <f t="shared" ref="Z17:Z23" si="4">IFERROR(Y17+Z16,"ERRO")</f>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="23:26">
@@ -14940,13 +14942,13 @@
         <f>SUMIF(Dados[Liquidez],W18,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y18" s="162" t="str">
+      <c r="Y18" s="162">
         <f t="shared" si="3"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z18" s="162" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="162">
         <f t="shared" si="4"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="23:26">
@@ -14955,13 +14957,13 @@
         <f>SUMIF(Dados[Liquidez],W19,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y19" s="164" t="str">
+      <c r="Y19" s="164">
         <f t="shared" si="3"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z19" s="164" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="164">
         <f t="shared" si="4"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="23:26">
@@ -14969,13 +14971,13 @@
         <f>SUMIF(Dados[Liquidez],W20,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y20" s="162" t="str">
+      <c r="Y20" s="162">
         <f t="shared" si="3"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z20" s="162" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="162">
         <f t="shared" si="4"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="23:26">
@@ -14984,13 +14986,13 @@
         <f>SUMIF(Dados[Liquidez],W21,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y21" s="164" t="str">
+      <c r="Y21" s="164">
         <f t="shared" si="3"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z21" s="164" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="164">
         <f t="shared" si="4"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="23:26">
@@ -14998,13 +15000,13 @@
         <f>SUMIF(Dados[Liquidez],W22,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y22" s="162" t="str">
+      <c r="Y22" s="162">
         <f t="shared" si="3"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z22" s="162" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="162">
         <f t="shared" si="4"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="23:26">
@@ -15013,13 +15015,13 @@
         <f>SUMIF(Dados[Liquidez],W23,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y23" s="164" t="str">
+      <c r="Y23" s="164">
         <f t="shared" si="3"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z23" s="164" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="164">
         <f t="shared" si="4"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="23:26">
@@ -15027,13 +15029,13 @@
         <f>SUMIF(Dados[Liquidez],W24,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y24" s="162" t="str">
+      <c r="Y24" s="162">
         <f t="shared" ref="Y24:Y29" si="5">IFERROR(X24/$Y$5,"ERRO")</f>
-        <v>ERRO</v>
-      </c>
-      <c r="Z24" s="162" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="162">
         <f t="shared" ref="Z24:Z29" si="6">IFERROR(Y24+Z23,"ERRO")</f>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="23:26">
@@ -15042,13 +15044,13 @@
         <f>SUMIF(Dados[Liquidez],W25,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y25" s="164" t="str">
+      <c r="Y25" s="164">
         <f t="shared" si="5"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z25" s="164" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="164">
         <f t="shared" si="6"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="23:26">
@@ -15056,13 +15058,13 @@
         <f>SUMIF(Dados[Liquidez],W26,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y26" s="162" t="str">
+      <c r="Y26" s="162">
         <f t="shared" si="5"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z26" s="162" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="162">
         <f t="shared" si="6"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="23:26">
@@ -15071,13 +15073,13 @@
         <f>SUMIF(Dados[Liquidez],W27,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y27" s="164" t="str">
+      <c r="Y27" s="164">
         <f t="shared" si="5"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z27" s="164" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="164">
         <f t="shared" si="6"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="23:26">
@@ -15085,13 +15087,13 @@
         <f>SUMIF(Dados[Liquidez],W28,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y28" s="162" t="str">
+      <c r="Y28" s="162">
         <f t="shared" si="5"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z28" s="162" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="162">
         <f t="shared" si="6"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="23:26">
@@ -15100,13 +15102,13 @@
         <f>SUMIF(Dados[Liquidez],W29,Dados[Saldo Bruto | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Y29" s="164" t="str">
+      <c r="Y29" s="164">
         <f t="shared" si="5"/>
-        <v>ERRO</v>
-      </c>
-      <c r="Z29" s="164" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="164">
         <f t="shared" si="6"/>
-        <v>ERRO</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -15438,15 +15440,15 @@
       <c r="N12" s="59"/>
       <c r="O12" s="8">
         <f>SUMIF(Dados[Classe],F12,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="P12" s="8">
         <f>SUMIF(Dados[Classe],F12,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="77" t="e">
+      <c r="Q12" s="77">
         <f>O12/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="R12" s="60"/>
       <c r="S12" s="9">
@@ -15457,7 +15459,7 @@
     <row r="13" spans="2:19">
       <c r="B13" s="156">
         <f>IFERROR(_xlfn.XLOOKUP(F13,ClasseSubClasse[SubClasse],ClasseSubClasse[Contagem]),"0")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C13" s="155">
         <v>1</v>
@@ -15484,15 +15486,15 @@
       <c r="N13" s="15"/>
       <c r="O13" s="62">
         <f>SUMIF(Dados[Subclasse],F13,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="P13" s="62">
         <f>SUMIF(Dados[Subclasse],F13,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="63" t="e">
+      <c r="Q13" s="63">
         <f>O13/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="R13" s="15"/>
       <c r="S13" s="64">
@@ -15527,15 +15529,15 @@
       <c r="N14" s="15"/>
       <c r="O14" s="11">
         <f>_xlfn.XLOOKUP(F14,Dados[Ativo],Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P14" s="11">
         <f>_xlfn.XLOOKUP(F14,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="222" t="e">
+      <c r="Q14" s="222">
         <f>O14/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R14" s="15"/>
       <c r="S14" s="150" t="str">
@@ -15569,15 +15571,15 @@
       <c r="N15" s="15"/>
       <c r="O15" s="10">
         <f>_xlfn.XLOOKUP(F15,Dados[Ativo],Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P15" s="10">
         <f>_xlfn.XLOOKUP(F15,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q15" s="66" t="e">
+      <c r="Q15" s="66">
         <f>O15/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R15" s="15"/>
       <c r="S15" s="13" t="str">
@@ -15611,15 +15613,15 @@
       <c r="N16" s="15"/>
       <c r="O16" s="69">
         <f>_xlfn.XLOOKUP(F16,Dados[Ativo],Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P16" s="69">
         <f>_xlfn.XLOOKUP(F16,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="70" t="e">
+      <c r="Q16" s="70">
         <f>O16/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R16" s="15"/>
       <c r="S16" s="71" t="str">
@@ -15663,20 +15665,20 @@
       <c r="N18" s="59"/>
       <c r="O18" s="8">
         <f>SUMIF(Dados[Classe],F18,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="P18" s="8">
         <f>SUMIF(Dados[Classe],F18,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="77" t="e">
+      <c r="Q18" s="77">
         <f>O18/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="R18" s="60"/>
       <c r="S18" s="9">
         <f>_xlfn.XLOOKUP(F18,Dados[Classe],Dados[Performance Classe])</f>
-        <v>0</v>
+        <v>-1.0985735394183094</v>
       </c>
     </row>
     <row r="19" spans="2:19">
@@ -15709,26 +15711,26 @@
       <c r="N19" s="15"/>
       <c r="O19" s="62">
         <f>SUMIF(Dados[Subclasse],F19,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="P19" s="62">
         <f>SUMIF(Dados[Subclasse],F19,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="63" t="e">
+      <c r="Q19" s="63">
         <f>O19/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="R19" s="15"/>
       <c r="S19" s="64">
         <f>_xlfn.XLOOKUP(F19,Dados[Subclasse],Dados[Performance SubClasse])</f>
-        <v>0</v>
+        <v>-1.0685262794319546</v>
       </c>
     </row>
     <row r="20" spans="2:19">
       <c r="F20" s="65" t="str" cm="1">
         <f t="array" ref="F20:F23">INDEX(_xlfn.SORTBY(_xlfn._xlws.FILTER(Dados[Ativo],(Dados[Subclasse]=F19)*(Dados[Lista?]=TRUE)),_xlfn._xlws.FILTER(Dados[Saldo Bruto | Mês Atual],(Dados[Subclasse]=F19)*(Dados[Lista?]=TRUE)),C19),_xlfn.SEQUENCE(D19))</f>
-        <v>CDB Bco. Master 12/28 16,10%aa</v>
+        <v>CDB Bco. Original 12/24 15,86%aa</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="79" t="str">
@@ -15743,34 +15745,34 @@
       <c r="K20" s="15"/>
       <c r="L20" s="10">
         <f>_xlfn.XLOOKUP(F20,Dados[Ativo],Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>125542.84</v>
+        <v>62610.36</v>
       </c>
       <c r="M20" s="66">
         <f>L20/SUM(Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>0.14274038257263719</v>
+        <v>7.1187068409560766E-2</v>
       </c>
       <c r="N20" s="15"/>
       <c r="O20" s="10">
         <f>_xlfn.XLOOKUP(F20,Dados[Ativo],Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P20" s="10">
         <f>_xlfn.XLOOKUP(F20,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="66" t="e">
+      <c r="Q20" s="66">
         <f>O20/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R20" s="15"/>
       <c r="S20" s="13">
         <f>_xlfn.XLOOKUP(F20,Dados[Ativo],Dados[Performance | Mês Atual])</f>
-        <v>-1</v>
+        <v>-0.9984028202361398</v>
       </c>
     </row>
     <row r="21" spans="2:19">
       <c r="F21" s="67" t="str">
-        <v>CDB Bco. Original 12/24 15,86%aa</v>
+        <v>CRA BTG Commodities 03/28 12,79%aa</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="80" t="str">
@@ -15785,34 +15787,34 @@
       <c r="K21" s="15"/>
       <c r="L21" s="69">
         <f>_xlfn.XLOOKUP(F21,Dados[Ativo],Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>62610.36</v>
+        <v>116012.23</v>
       </c>
       <c r="M21" s="70">
         <f>L21/SUM(Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>7.1187068409560766E-2</v>
+        <v>0.13190421766231175</v>
       </c>
       <c r="N21" s="15"/>
       <c r="O21" s="69">
         <f>_xlfn.XLOOKUP(F21,Dados[Ativo],Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P21" s="69">
         <f>_xlfn.XLOOKUP(F21,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q21" s="70" t="e">
+      <c r="Q21" s="70">
         <f>O21/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R21" s="15"/>
       <c r="S21" s="71">
         <f>_xlfn.XLOOKUP(F21,Dados[Ativo],Dados[Performance | Mês Atual])</f>
-        <v>-1</v>
+        <v>-1.1754564963690872</v>
       </c>
     </row>
     <row r="22" spans="2:19">
       <c r="F22" s="223" t="str">
-        <v>CRA BTG Commodities 03/28 12,79%aa</v>
+        <v>CRA Engelhart CTP 01/28 13,58%aa</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="79" t="str">
@@ -15827,34 +15829,34 @@
       <c r="K22" s="15"/>
       <c r="L22" s="10">
         <f>_xlfn.XLOOKUP(F22,Dados[Ativo],Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>116012.23</v>
+        <v>26072.27</v>
       </c>
       <c r="M22" s="66">
         <f>L22/SUM(Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>0.13190421766231175</v>
+        <v>2.9643791667745382E-2</v>
       </c>
       <c r="N22" s="15"/>
       <c r="O22" s="10">
         <f>_xlfn.XLOOKUP(F22,Dados[Ativo],Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P22" s="10">
         <f>_xlfn.XLOOKUP(F22,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="66" t="e">
+      <c r="Q22" s="66">
         <f>O22/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R22" s="15"/>
       <c r="S22" s="13">
         <f>_xlfn.XLOOKUP(F22,Dados[Ativo],Dados[Performance | Mês Atual])</f>
-        <v>-1.1764705882352942</v>
+        <v>-1.1719582439390925</v>
       </c>
     </row>
     <row r="23" spans="2:19">
       <c r="F23" s="67" t="str">
-        <v>CRA Engelhart CTP 01/28 13,58%aa</v>
+        <v>CDB Bco. Master 12/28 16,10%aa</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="80" t="str">
@@ -15869,29 +15871,29 @@
       <c r="K23" s="15"/>
       <c r="L23" s="69">
         <f>_xlfn.XLOOKUP(F23,Dados[Ativo],Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>26072.27</v>
+        <v>125542.84</v>
       </c>
       <c r="M23" s="70">
         <f>L23/SUM(Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>2.9643791667745382E-2</v>
+        <v>0.14274038257263719</v>
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="69">
         <f>_xlfn.XLOOKUP(F23,Dados[Ativo],Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P23" s="69">
         <f>_xlfn.XLOOKUP(F23,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="70" t="e">
+      <c r="Q23" s="70">
         <f>O23/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="R23" s="15"/>
       <c r="S23" s="71">
         <f>_xlfn.XLOOKUP(F23,Dados[Ativo],Dados[Performance | Mês Atual])</f>
-        <v>-1.1764705882352942</v>
+        <v>-0.99840691830772665</v>
       </c>
     </row>
     <row r="24" spans="2:19" ht="4.5" customHeight="1">
@@ -15940,26 +15942,26 @@
       <c r="N25" s="15"/>
       <c r="O25" s="62">
         <f>SUMIF(Dados[Subclasse],F25,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P25" s="62">
         <f>SUMIF(Dados[Subclasse],F25,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q25" s="63" t="e">
+      <c r="Q25" s="63">
         <f>O25/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="R25" s="15"/>
       <c r="S25" s="64">
         <f>_xlfn.XLOOKUP(F25,Dados[Subclasse],Dados[Performance SubClasse])</f>
-        <v>0</v>
+        <v>-1.1736916893841964</v>
       </c>
     </row>
     <row r="26" spans="2:19">
       <c r="F26" s="65" t="str" cm="1">
         <f t="array" ref="F26:F28">INDEX(_xlfn.SORTBY(_xlfn._xlws.FILTER(Dados[Ativo],(Dados[Subclasse]=F25)*(Dados[Lista?]=TRUE)),_xlfn._xlws.FILTER(Dados[Saldo Bruto | Mês Atual],(Dados[Subclasse]=F25)*(Dados[Lista?]=TRUE)),C25),_xlfn.SEQUENCE(D25))</f>
-        <v>CRA Eldorado 09/27 IPCA+ 6,20%aa</v>
+        <v>Deb. Via Brasil 12/30 IPCA+ 9,11%aa</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="79" t="str">
@@ -15974,11 +15976,11 @@
       <c r="K26" s="15"/>
       <c r="L26" s="10">
         <f>_xlfn.XLOOKUP(F26,Dados[Ativo],Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>110292.68</v>
+        <v>113824.9</v>
       </c>
       <c r="M26" s="66">
         <f>L26/SUM(Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>0.12540117252534236</v>
+        <v>0.12941725527550732</v>
       </c>
       <c r="N26" s="15"/>
       <c r="O26" s="10">
@@ -15989,9 +15991,9 @@
         <f>_xlfn.XLOOKUP(F26,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q26" s="66" t="e">
+      <c r="Q26" s="66">
         <f>O26/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="R26" s="15"/>
       <c r="S26" s="13">
@@ -16001,7 +16003,7 @@
     </row>
     <row r="27" spans="2:19">
       <c r="F27" s="67" t="str">
-        <v>Deb. Enauta 12/29 IPCA+ 9,46%aa</v>
+        <v>CRA Eldorado 09/27 IPCA+ 6,20%aa</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="80" t="str">
@@ -16016,34 +16018,34 @@
       <c r="K27" s="15"/>
       <c r="L27" s="69">
         <f>_xlfn.XLOOKUP(F27,Dados[Ativo],Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>26195.5</v>
+        <v>110292.68</v>
       </c>
       <c r="M27" s="70">
         <f>L27/SUM(Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>2.9783902384887245E-2</v>
+        <v>0.12540117252534236</v>
       </c>
       <c r="N27" s="15"/>
       <c r="O27" s="69">
         <f>_xlfn.XLOOKUP(F27,Dados[Ativo],Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P27" s="69">
         <f>_xlfn.XLOOKUP(F27,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q27" s="70" t="e">
+      <c r="Q27" s="70">
         <f>O27/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R27" s="15"/>
       <c r="S27" s="71">
         <f>_xlfn.XLOOKUP(F27,Dados[Ativo],Dados[Performance | Mês Atual])</f>
-        <v>-1.1764705882352942</v>
+        <v>-1.1754039076648017</v>
       </c>
     </row>
     <row r="28" spans="2:19">
       <c r="F28" s="65" t="str">
-        <v>Deb. Via Brasil 12/30 IPCA+ 9,11%aa</v>
+        <v>Deb. Enauta 12/29 IPCA+ 9,46%aa</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="79" t="str">
@@ -16058,29 +16060,29 @@
       <c r="K28" s="15"/>
       <c r="L28" s="10">
         <f>_xlfn.XLOOKUP(F28,Dados[Ativo],Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>113824.9</v>
+        <v>26195.5</v>
       </c>
       <c r="M28" s="66">
         <f>L28/SUM(Dados[Saldo Bruto | Mês Anterior])</f>
-        <v>0.12941725527550732</v>
+        <v>2.9783902384887245E-2</v>
       </c>
       <c r="N28" s="15"/>
       <c r="O28" s="10">
         <f>_xlfn.XLOOKUP(F28,Dados[Ativo],Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P28" s="10">
         <f>_xlfn.XLOOKUP(F28,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q28" s="66" t="e">
+      <c r="Q28" s="66">
         <f>O28/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R28" s="15"/>
       <c r="S28" s="13">
         <f>_xlfn.XLOOKUP(F28,Dados[Ativo],Dados[Performance | Mês Atual])</f>
-        <v>-1.1764705882352942</v>
+        <v>-1.1719794711035911</v>
       </c>
     </row>
     <row r="29" spans="2:19" ht="4.5" customHeight="1" thickBot="1">
@@ -16119,20 +16121,20 @@
       <c r="N30" s="59"/>
       <c r="O30" s="8">
         <f>SUMIF(Dados[Classe],F30,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P30" s="8">
         <f>SUMIF(Dados[Classe],F30,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q30" s="77" t="e">
+      <c r="Q30" s="77">
         <f>O30/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R30" s="60"/>
       <c r="S30" s="9">
         <f>_xlfn.XLOOKUP(F30,Dados[Classe],Dados[Performance Classe])</f>
-        <v>0</v>
+        <v>-0.99847249326980536</v>
       </c>
     </row>
     <row r="31" spans="2:19">
@@ -16165,20 +16167,20 @@
       <c r="N31" s="15"/>
       <c r="O31" s="62">
         <f>SUMIF(Dados[Subclasse],F31,Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P31" s="62">
         <f>SUMIF(Dados[Subclasse],F31,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q31" s="63" t="e">
+      <c r="Q31" s="63">
         <f>O31/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R31" s="15"/>
       <c r="S31" s="64">
         <f>_xlfn.XLOOKUP(F31,Dados[Subclasse],Dados[Performance SubClasse])</f>
-        <v>0</v>
+        <v>-0.99847249326980536</v>
       </c>
     </row>
     <row r="32" spans="2:19">
@@ -16208,20 +16210,20 @@
       <c r="N32" s="15"/>
       <c r="O32" s="69">
         <f>_xlfn.XLOOKUP(F32,Dados[Ativo],Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P32" s="69">
         <f>_xlfn.XLOOKUP(F32,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q32" s="70" t="e">
+      <c r="Q32" s="70">
         <f>O32/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="R32" s="15"/>
       <c r="S32" s="71">
         <f>_xlfn.XLOOKUP(F32,Dados[Ativo],Dados[Performance | Mês Atual])</f>
-        <v>-1</v>
+        <v>-0.99847249326980536</v>
       </c>
     </row>
     <row r="33" spans="2:23" ht="4.5" customHeight="1" thickBot="1">
@@ -16266,9 +16268,9 @@
         <f>SUMIF(Dados[Classe],F34,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q34" s="77" t="e">
+      <c r="Q34" s="77">
         <f>O34/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="R34" s="60"/>
       <c r="S34" s="9">
@@ -16312,9 +16314,9 @@
         <f>SUMIF(Dados[Subclasse],F35,Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q35" s="63" t="e">
+      <c r="Q35" s="63">
         <f>O35/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="R35" s="15"/>
       <c r="S35" s="64">
@@ -16355,9 +16357,9 @@
         <f>_xlfn.XLOOKUP(F36,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q36" s="66" t="e">
+      <c r="Q36" s="66">
         <f>O36/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="R36" s="15"/>
       <c r="S36" s="13">
@@ -16397,9 +16399,9 @@
         <f>_xlfn.XLOOKUP(F37,Dados[Ativo],Dados[Movimentaçao | Mês Atual])</f>
         <v>0</v>
       </c>
-      <c r="Q37" s="70" t="e">
+      <c r="Q37" s="70">
         <f>O37/SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="R37" s="15"/>
       <c r="S37" s="71">
@@ -16481,7 +16483,7 @@
       </c>
       <c r="O40" s="85">
         <f>SUM(Dados[Saldo Bruto | Mês Atual])</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="P40" s="85">
         <f>SUM(Dados[Movimentaçao | Mês Atual])</f>
@@ -16617,8 +16619,8 @@
   <dimension ref="A1:BS28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B8" sqref="B8"/>
+      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16781,7 +16783,7 @@
       </c>
       <c r="AD2" s="58">
         <f>SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira])</f>
-        <v>0</v>
+        <v>-0.78986247901799733</v>
       </c>
       <c r="AE2" s="56"/>
       <c r="AF2" s="56"/>
@@ -17099,7 +17101,7 @@
       <c r="BR5" s="50"/>
       <c r="BS5" s="50"/>
     </row>
-    <row r="6" spans="1:71" ht="11.25" hidden="1">
+    <row r="6" spans="1:71" ht="11.25">
       <c r="B6" s="157" t="str">
         <f>IF(Dados[[#This Row],[Tipo do Ativo]]="","",Dados[[#This Row],[Tipo do Ativo]]&amp;" ")&amp;IF(Dados[[#This Row],[Emissor]]="","",Dados[[#This Row],[Emissor]])&amp;IF(Dados[[#This Row],[Vencimento]]="",""," "&amp;TEXT(Dados[[#This Row],[Vencimento]],"mm/aa"))&amp;IF(Dados[[#This Row],[Remuneração]]="",""," "&amp;TEXT(Dados[[#This Row],[Remuneração]],"##,##%"))&amp;IF(Dados[[#This Row],[Complemento]]="",""," "&amp;Dados[[#This Row],[Complemento]])</f>
         <v>BTG CDB Plus FI RF CP</v>
@@ -17156,14 +17158,18 @@
         <f t="array" ref="Y6">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z6" s="55">
-        <v>100</v>
+      <c r="Z6" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA6" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC6" s="56">
+      <c r="AC6" s="245">
+        <v>200</v>
+      </c>
+      <c r="AD6" s="243">
         <v>100</v>
       </c>
       <c r="AE6" s="56"/>
@@ -17189,9 +17195,9 @@
       <c r="AQ6" s="56">
         <v>120</v>
       </c>
-      <c r="AS6" s="51" t="str">
+      <c r="AS6" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AT6" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
@@ -17199,15 +17205,15 @@
       </c>
       <c r="AU6" s="180">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
-        <v>-1</v>
+        <v>-0.99847249326980536</v>
       </c>
       <c r="AV6" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="AW6" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AX6" s="56">
         <f>SUM(Dados[[#This Row],[Aplicações]:[Cashback]])</f>
@@ -17225,39 +17231,39 @@
       <c r="BB6" s="56"/>
       <c r="BC6" s="56">
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD6" s="51" t="str">
+        <v>100</v>
+      </c>
+      <c r="BD6" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="BE6" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF6" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF6" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="BG6" s="51" cm="1">
         <f t="array" ref="BG6">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BH6" s="51" t="str">
+        <v>-0.96538747435533001</v>
+      </c>
+      <c r="BH6" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>1</v>
       </c>
       <c r="BI6" s="51" cm="1">
         <f t="array" ref="BI6">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BJ6" s="51" t="str">
+        <v>-0.99847249326980536</v>
+      </c>
+      <c r="BJ6" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>1</v>
       </c>
       <c r="BK6" s="51" cm="1">
         <f t="array" ref="BK6">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
-        <v>0</v>
+        <v>-0.99847249326980536</v>
       </c>
       <c r="BL6" s="51"/>
       <c r="BN6" s="50"/>
@@ -17331,14 +17337,20 @@
         <f t="array" ref="Y7">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z7" s="55">
-        <v>200</v>
+      <c r="Z7" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA7" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC7" s="56"/>
+      <c r="AC7" s="242">
+        <v>200</v>
+      </c>
+      <c r="AD7" s="243">
+        <v>200</v>
+      </c>
       <c r="AE7" s="56"/>
       <c r="AF7" s="56"/>
       <c r="AI7" s="56"/>
@@ -17362,9 +17374,9 @@
       <c r="AQ7" s="56">
         <v>0</v>
       </c>
-      <c r="AS7" s="51" t="str">
+      <c r="AS7" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="AT7" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
@@ -17372,15 +17384,15 @@
       </c>
       <c r="AU7" s="180">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
-        <v>-1</v>
+        <v>-0.99840691830772665</v>
       </c>
       <c r="AV7" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW7" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AX7" s="56">
         <f>SUM(Dados[[#This Row],[Aplicações]:[Cashback]])</f>
@@ -17398,39 +17410,39 @@
       <c r="BB7" s="56"/>
       <c r="BC7" s="56">
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD7" s="51" t="str">
+        <v>200</v>
+      </c>
+      <c r="BD7" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="BE7" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF7" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF7" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="BG7" s="51" cm="1">
         <f t="array" ref="BG7">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BH7" s="51" t="str">
+        <v>-0.96538747435533001</v>
+      </c>
+      <c r="BH7" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.4</v>
       </c>
       <c r="BI7" s="51" cm="1">
         <f t="array" ref="BI7">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BJ7" s="51" t="str">
+        <v>-1.0685262794319546</v>
+      </c>
+      <c r="BJ7" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="BK7" s="51" cm="1">
         <f t="array" ref="BK7">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
-        <v>0</v>
+        <v>-1.0985735394183094</v>
       </c>
       <c r="BL7" s="51"/>
       <c r="BN7" s="50"/>
@@ -17504,14 +17516,20 @@
         <f t="array" ref="Y8">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z8" s="55">
-        <v>300</v>
+      <c r="Z8" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA8" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC8" s="56"/>
+      <c r="AC8" s="245">
+        <v>300</v>
+      </c>
+      <c r="AD8" s="243">
+        <v>100</v>
+      </c>
       <c r="AE8" s="56"/>
       <c r="AF8" s="56"/>
       <c r="AI8" s="56"/>
@@ -17535,25 +17553,25 @@
       <c r="AQ8" s="56">
         <v>0</v>
       </c>
-      <c r="AS8" s="51" t="str">
+      <c r="AS8" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AT8" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="AU8" s="180">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
-        <v>-1</v>
+        <v>-0.9984028202361398</v>
       </c>
       <c r="AV8" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="AW8" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AX8" s="56">
         <f>SUM(Dados[[#This Row],[Aplicações]:[Cashback]])</f>
@@ -17571,39 +17589,39 @@
       <c r="BB8" s="56"/>
       <c r="BC8" s="56">
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD8" s="51" t="str">
+        <v>100</v>
+      </c>
+      <c r="BD8" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="BE8" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF8" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF8" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="BG8" s="51" cm="1">
         <f t="array" ref="BG8">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BH8" s="51" t="str">
+        <v>-0.96538747435533001</v>
+      </c>
+      <c r="BH8" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.2</v>
       </c>
       <c r="BI8" s="51" cm="1">
         <f t="array" ref="BI8">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="51" t="str">
+        <v>-1.0685262794319546</v>
+      </c>
+      <c r="BJ8" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="BK8" s="51" cm="1">
         <f t="array" ref="BK8">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
-        <v>0</v>
+        <v>-1.0985735394183094</v>
       </c>
       <c r="BL8" s="51"/>
       <c r="BN8" s="50"/>
@@ -17611,7 +17629,7 @@
       <c r="BR8" s="50"/>
       <c r="BS8" s="50"/>
     </row>
-    <row r="9" spans="1:71" ht="11.25" hidden="1">
+    <row r="9" spans="1:71" ht="11.25">
       <c r="B9" s="157" t="str">
         <f>IF(Dados[[#This Row],[Tipo do Ativo]]="","",Dados[[#This Row],[Tipo do Ativo]]&amp;" ")&amp;IF(Dados[[#This Row],[Emissor]]="","",Dados[[#This Row],[Emissor]])&amp;IF(Dados[[#This Row],[Vencimento]]="",""," "&amp;TEXT(Dados[[#This Row],[Vencimento]],"mm/aa"))&amp;IF(Dados[[#This Row],[Remuneração]]="",""," "&amp;TEXT(Dados[[#This Row],[Remuneração]],"##,##%"))&amp;IF(Dados[[#This Row],[Complemento]]="",""," "&amp;Dados[[#This Row],[Complemento]])</f>
         <v>Conta Corrente - BTG</v>
@@ -17668,14 +17686,20 @@
         <f t="array" ref="Y9">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z9" s="55">
-        <v>400</v>
+      <c r="Z9" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA9" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC9" s="56"/>
+      <c r="AC9" s="242">
+        <v>200</v>
+      </c>
+      <c r="AD9" s="243">
+        <v>100</v>
+      </c>
       <c r="AE9" s="56"/>
       <c r="AF9" s="56"/>
       <c r="AI9" s="56"/>
@@ -17699,13 +17723,13 @@
       <c r="AQ9" s="56">
         <v>0</v>
       </c>
-      <c r="AS9" s="51" t="str">
+      <c r="AS9" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AT9" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AU9" s="180" t="str">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
@@ -17713,11 +17737,11 @@
       </c>
       <c r="AV9" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW9" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AX9" s="56">
         <f>SUM(Dados[[#This Row],[Aplicações]:[Cashback]])</f>
@@ -17730,40 +17754,40 @@
       <c r="AZ9" s="50"/>
       <c r="BA9" s="50" t="b">
         <f>OR(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]&lt;&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]]&lt;&gt;0,Dados[[#This Row],[Movimentaçao | Mês Atual]]&lt;&gt;0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB9" s="56"/>
       <c r="BC9" s="56">
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD9" s="51" t="str">
+        <v>100</v>
+      </c>
+      <c r="BD9" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="BE9" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF9" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF9" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="BG9" s="51" cm="1">
         <f t="array" ref="BG9">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BH9" s="51" t="str">
+        <v>-0.96538747435533001</v>
+      </c>
+      <c r="BH9" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="BI9" s="51" cm="1">
         <f t="array" ref="BI9">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
         <v>0</v>
       </c>
-      <c r="BJ9" s="51" t="str">
+      <c r="BJ9" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="BK9" s="51" cm="1">
         <f t="array" ref="BK9">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
@@ -17775,7 +17799,7 @@
       <c r="BR9" s="50"/>
       <c r="BS9" s="50"/>
     </row>
-    <row r="10" spans="1:71" ht="11.25" hidden="1">
+    <row r="10" spans="1:71" ht="11.25">
       <c r="B10" s="157" t="str">
         <f>IF(Dados[[#This Row],[Tipo do Ativo]]="","",Dados[[#This Row],[Tipo do Ativo]]&amp;" ")&amp;IF(Dados[[#This Row],[Emissor]]="","",Dados[[#This Row],[Emissor]])&amp;IF(Dados[[#This Row],[Vencimento]]="",""," "&amp;TEXT(Dados[[#This Row],[Vencimento]],"mm/aa"))&amp;IF(Dados[[#This Row],[Remuneração]]="",""," "&amp;TEXT(Dados[[#This Row],[Remuneração]],"##,##%"))&amp;IF(Dados[[#This Row],[Complemento]]="",""," "&amp;Dados[[#This Row],[Complemento]])</f>
         <v>Conta Corrente - Safra</v>
@@ -17832,18 +17856,19 @@
         <f t="array" ref="Y10">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z10" s="55">
-        <v>500</v>
+      <c r="Z10" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA10" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC10" s="220">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="220">
-        <v>0</v>
+      <c r="AC10" s="242">
+        <v>200</v>
+      </c>
+      <c r="AD10" s="244">
+        <v>100</v>
       </c>
       <c r="AE10" s="56"/>
       <c r="AF10" s="56"/>
@@ -17868,13 +17893,13 @@
       <c r="AQ10" s="56">
         <v>0</v>
       </c>
-      <c r="AS10" s="51" t="str">
+      <c r="AS10" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AT10" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AU10" s="180" t="str">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
@@ -17882,11 +17907,11 @@
       </c>
       <c r="AV10" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW10" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AX10" s="56">
         <f>SUM(Dados[[#This Row],[Aplicações]:[Cashback]])</f>
@@ -17899,40 +17924,40 @@
       <c r="AZ10" s="50"/>
       <c r="BA10" s="50" t="b">
         <f>OR(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]&lt;&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]]&lt;&gt;0,Dados[[#This Row],[Movimentaçao | Mês Atual]]&lt;&gt;0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB10" s="56"/>
       <c r="BC10" s="56">
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD10" s="51" t="str">
+        <v>100</v>
+      </c>
+      <c r="BD10" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="BE10" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF10" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF10" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>1</v>
       </c>
       <c r="BG10" s="51" cm="1">
         <f t="array" ref="BG10">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
         <v>0</v>
       </c>
-      <c r="BH10" s="51" t="str">
+      <c r="BH10" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="BI10" s="51" cm="1">
         <f t="array" ref="BI10">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
         <v>0</v>
       </c>
-      <c r="BJ10" s="51" t="str">
+      <c r="BJ10" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="BK10" s="51" cm="1">
         <f t="array" ref="BK10">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
@@ -17944,7 +17969,7 @@
       <c r="BR10" s="50"/>
       <c r="BS10" s="50"/>
     </row>
-    <row r="11" spans="1:71" ht="11.25" hidden="1">
+    <row r="11" spans="1:71" ht="11.25">
       <c r="B11" s="157" t="str">
         <f>IF(Dados[[#This Row],[Tipo do Ativo]]="","",Dados[[#This Row],[Tipo do Ativo]]&amp;" ")&amp;IF(Dados[[#This Row],[Emissor]]="","",Dados[[#This Row],[Emissor]])&amp;IF(Dados[[#This Row],[Vencimento]]="",""," "&amp;TEXT(Dados[[#This Row],[Vencimento]],"mm/aa"))&amp;IF(Dados[[#This Row],[Remuneração]]="",""," "&amp;TEXT(Dados[[#This Row],[Remuneração]],"##,##%"))&amp;IF(Dados[[#This Row],[Complemento]]="",""," "&amp;Dados[[#This Row],[Complemento]])</f>
         <v>Conta Corrente - Santander</v>
@@ -18001,18 +18026,19 @@
         <f t="array" ref="Y11">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z11" s="55">
-        <v>600</v>
+      <c r="Z11" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA11" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC11" s="220">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="220">
-        <v>0</v>
+      <c r="AC11" s="242">
+        <v>200</v>
+      </c>
+      <c r="AD11" s="244">
+        <v>100</v>
       </c>
       <c r="AE11" s="56"/>
       <c r="AF11" s="56"/>
@@ -18037,13 +18063,13 @@
       <c r="AQ11" s="56">
         <v>0</v>
       </c>
-      <c r="AS11" s="51" t="str">
+      <c r="AS11" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AT11" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AU11" s="180" t="str">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
@@ -18051,11 +18077,11 @@
       </c>
       <c r="AV11" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW11" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AX11" s="56">
         <f>SUM(Dados[[#This Row],[Aplicações]:[Cashback]])</f>
@@ -18068,40 +18094,40 @@
       <c r="AZ11" s="50"/>
       <c r="BA11" s="50" t="b">
         <f>OR(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]&lt;&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]]&lt;&gt;0,Dados[[#This Row],[Movimentaçao | Mês Atual]]&lt;&gt;0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB11" s="56"/>
       <c r="BC11" s="56">
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD11" s="51" t="str">
+        <v>100</v>
+      </c>
+      <c r="BD11" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="BE11" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF11" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF11" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>1</v>
       </c>
       <c r="BG11" s="51" cm="1">
         <f t="array" ref="BG11">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
         <v>0</v>
       </c>
-      <c r="BH11" s="51" t="str">
+      <c r="BH11" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="BI11" s="51" cm="1">
         <f t="array" ref="BI11">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
         <v>0</v>
       </c>
-      <c r="BJ11" s="51" t="str">
+      <c r="BJ11" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="BK11" s="51" cm="1">
         <f t="array" ref="BK11">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
@@ -18182,14 +18208,20 @@
         <f t="array" ref="Y12">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z12" s="55">
-        <v>700</v>
+      <c r="Z12" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA12" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC12" s="56"/>
+      <c r="AC12" s="242">
+        <v>200</v>
+      </c>
+      <c r="AD12" s="243">
+        <v>100</v>
+      </c>
       <c r="AE12" s="56"/>
       <c r="AF12" s="56"/>
       <c r="AI12" s="56"/>
@@ -18213,25 +18245,25 @@
       <c r="AQ12" s="56">
         <v>0</v>
       </c>
-      <c r="AS12" s="51" t="str">
+      <c r="AS12" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AT12" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AU12" s="180">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
-        <v>-1.1764705882352942</v>
+        <v>-1.1754564963690872</v>
       </c>
       <c r="AV12" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW12" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AX12" s="56">
         <f>SUM(Dados[[#This Row],[Aplicações]:[Cashback]])</f>
@@ -18249,39 +18281,39 @@
       <c r="BB12" s="56"/>
       <c r="BC12" s="56">
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD12" s="51" t="str">
+        <v>100</v>
+      </c>
+      <c r="BD12" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="BE12" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF12" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF12" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="BG12" s="51" cm="1">
         <f t="array" ref="BG12">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BH12" s="51" t="str">
+        <v>-0.96538747435533001</v>
+      </c>
+      <c r="BH12" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.2</v>
       </c>
       <c r="BI12" s="51" cm="1">
         <f t="array" ref="BI12">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BJ12" s="51" t="str">
+        <v>-1.0685262794319546</v>
+      </c>
+      <c r="BJ12" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="BK12" s="51" cm="1">
         <f t="array" ref="BK12">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
-        <v>0</v>
+        <v>-1.0985735394183094</v>
       </c>
       <c r="BL12" s="51"/>
       <c r="BN12" s="50"/>
@@ -18358,14 +18390,20 @@
         <f t="array" ref="Y13">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z13" s="55">
-        <v>5</v>
+      <c r="Z13" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA13" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC13" s="56"/>
+      <c r="AC13" s="242">
+        <v>200</v>
+      </c>
+      <c r="AD13" s="243">
+        <v>100</v>
+      </c>
       <c r="AE13" s="56"/>
       <c r="AF13" s="56"/>
       <c r="AI13" s="56"/>
@@ -18389,25 +18427,25 @@
       <c r="AQ13" s="56">
         <v>0</v>
       </c>
-      <c r="AS13" s="51" t="str">
+      <c r="AS13" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AT13" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AU13" s="180">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
-        <v>-1.1764705882352942</v>
+        <v>-1.1754039076648017</v>
       </c>
       <c r="AV13" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW13" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AX13" s="56">
         <f>SUM(Dados[[#This Row],[Aplicações]:[Cashback]])</f>
@@ -18425,39 +18463,39 @@
       <c r="BB13" s="56"/>
       <c r="BC13" s="56">
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD13" s="51" t="str">
+        <v>100</v>
+      </c>
+      <c r="BD13" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="BE13" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF13" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF13" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="BG13" s="51" cm="1">
         <f t="array" ref="BG13">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BH13" s="51" t="str">
+        <v>-0.96538747435533001</v>
+      </c>
+      <c r="BH13" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.5</v>
       </c>
       <c r="BI13" s="51" cm="1">
         <f t="array" ref="BI13">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BJ13" s="51" t="str">
+        <v>-1.1736916893841964</v>
+      </c>
+      <c r="BJ13" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="BK13" s="51" cm="1">
         <f t="array" ref="BK13">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
-        <v>0</v>
+        <v>-1.0985735394183094</v>
       </c>
       <c r="BL13" s="51"/>
       <c r="BN13" s="50"/>
@@ -18534,14 +18572,20 @@
         <f t="array" ref="Y14">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z14" s="55">
-        <v>30</v>
+      <c r="Z14" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA14" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC14" s="56"/>
+      <c r="AC14" s="242">
+        <v>200</v>
+      </c>
+      <c r="AD14" s="243">
+        <v>100</v>
+      </c>
       <c r="AE14" s="56"/>
       <c r="AF14" s="56"/>
       <c r="AI14" s="56"/>
@@ -18565,25 +18609,25 @@
       <c r="AQ14" s="56">
         <v>0</v>
       </c>
-      <c r="AS14" s="51" t="str">
+      <c r="AS14" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AT14" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AU14" s="180">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
-        <v>-1.1764705882352942</v>
+        <v>-1.1719582439390925</v>
       </c>
       <c r="AV14" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW14" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AX14" s="56">
         <f>SUM(Dados[[#This Row],[Aplicações]:[Cashback]])</f>
@@ -18601,39 +18645,39 @@
       <c r="BB14" s="56"/>
       <c r="BC14" s="56">
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD14" s="51" t="str">
+        <v>100</v>
+      </c>
+      <c r="BD14" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="BE14" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF14" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF14" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="BG14" s="51" cm="1">
         <f t="array" ref="BG14">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BH14" s="51" t="str">
+        <v>-0.96538747435533001</v>
+      </c>
+      <c r="BH14" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.2</v>
       </c>
       <c r="BI14" s="51" cm="1">
         <f t="array" ref="BI14">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BJ14" s="51" t="str">
+        <v>-1.0685262794319546</v>
+      </c>
+      <c r="BJ14" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="BK14" s="51" cm="1">
         <f t="array" ref="BK14">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
-        <v>0</v>
+        <v>-1.0985735394183094</v>
       </c>
       <c r="BL14" s="51"/>
       <c r="BN14" s="50"/>
@@ -18710,14 +18754,20 @@
         <f t="array" ref="Y15">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z15" s="55">
-        <v>30</v>
+      <c r="Z15" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA15" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC15" s="56"/>
+      <c r="AC15" s="242">
+        <v>200</v>
+      </c>
+      <c r="AD15" s="243">
+        <v>100</v>
+      </c>
       <c r="AE15" s="56"/>
       <c r="AF15" s="56"/>
       <c r="AI15" s="56"/>
@@ -18741,25 +18791,25 @@
       <c r="AQ15" s="56">
         <v>0</v>
       </c>
-      <c r="AS15" s="51" t="str">
+      <c r="AS15" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AT15" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AU15" s="180">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
-        <v>-1.1764705882352942</v>
+        <v>-1.1719794711035911</v>
       </c>
       <c r="AV15" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW15" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AX15" s="56">
         <f>SUM(Dados[[#This Row],[Aplicações]:[Cashback]])</f>
@@ -18777,39 +18827,39 @@
       <c r="BB15" s="56"/>
       <c r="BC15" s="56">
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD15" s="51" t="str">
+        <v>100</v>
+      </c>
+      <c r="BD15" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="BE15" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF15" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF15" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="BG15" s="51" cm="1">
         <f t="array" ref="BG15">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BH15" s="51" t="str">
+        <v>-0.96538747435533001</v>
+      </c>
+      <c r="BH15" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.5</v>
       </c>
       <c r="BI15" s="51" cm="1">
         <f t="array" ref="BI15">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BJ15" s="51" t="str">
+        <v>-1.1736916893841964</v>
+      </c>
+      <c r="BJ15" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="BK15" s="51" cm="1">
         <f t="array" ref="BK15">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
-        <v>0</v>
+        <v>-1.0985735394183094</v>
       </c>
       <c r="BL15" s="51"/>
       <c r="BN15" s="50"/>
@@ -18886,14 +18936,17 @@
         <f t="array" ref="Y16">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z16" s="55">
-        <v>30</v>
+      <c r="Z16" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA16" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC16" s="56"/>
+      <c r="AC16" s="245">
+        <v>200</v>
+      </c>
       <c r="AE16" s="56"/>
       <c r="AF16" s="56"/>
       <c r="AI16" s="56"/>
@@ -18917,13 +18970,13 @@
       <c r="AQ16" s="56">
         <v>0</v>
       </c>
-      <c r="AS16" s="51" t="str">
+      <c r="AS16" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="AT16" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="AU16" s="180">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
@@ -18931,7 +18984,7 @@
       </c>
       <c r="AV16" s="56">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW16" s="56">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
@@ -18955,37 +19008,37 @@
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
         <v>0</v>
       </c>
-      <c r="BD16" s="51" t="str">
+      <c r="BD16" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BE16" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF16" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF16" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BG16" s="51" cm="1">
         <f t="array" ref="BG16">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BH16" s="51" t="str">
+        <v>-0.96538747435533001</v>
+      </c>
+      <c r="BH16" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BI16" s="51" cm="1">
         <f t="array" ref="BI16">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | SubClasse],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Subclasse]=Dados[[#This Row],[Subclasse]])),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BJ16" s="51" t="str">
+        <v>-1.1736916893841964</v>
+      </c>
+      <c r="BJ16" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Classe],Dados[[#This Row],[Classe]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BK16" s="51" cm="1">
         <f t="array" ref="BK16">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Classe],Dados[Classe]=Dados[[#This Row],[Classe]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Classe]=Dados[[#This Row],[Classe]])),"0,00%")</f>
-        <v>0</v>
+        <v>-1.0985735394183094</v>
       </c>
       <c r="BL16" s="51"/>
       <c r="BN16" s="50"/>
@@ -19050,15 +19103,16 @@
         <f t="array" ref="Y17">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z17" s="55">
-        <v>30</v>
+      <c r="Z17" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA17" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC17" s="220">
-        <v>0</v>
+      <c r="AC17" s="245">
+        <v>200</v>
       </c>
       <c r="AD17" s="220">
         <v>0</v>
@@ -19089,13 +19143,13 @@
       <c r="AQ17" s="227">
         <v>0</v>
       </c>
-      <c r="AS17" s="225" t="str">
+      <c r="AS17" s="225">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="AT17" s="227">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="AU17" s="226" t="str">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
@@ -19103,7 +19157,7 @@
       </c>
       <c r="AV17" s="227">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW17" s="227">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
@@ -19127,17 +19181,17 @@
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
         <v>0</v>
       </c>
-      <c r="BD17" s="225" t="str">
+      <c r="BD17" s="225">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BE17" s="225">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF17" s="225" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF17" s="225">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BG17" s="225" cm="1">
         <f t="array" ref="BG17">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
@@ -19222,15 +19276,16 @@
         <f t="array" ref="Y18">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z18" s="55">
-        <v>30</v>
+      <c r="Z18" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA18" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
         <v/>
       </c>
-      <c r="AC18" s="220">
-        <v>0</v>
+      <c r="AC18" s="245">
+        <v>200</v>
       </c>
       <c r="AD18" s="220">
         <v>0</v>
@@ -19261,13 +19316,13 @@
       <c r="AQ18" s="227">
         <v>0</v>
       </c>
-      <c r="AS18" s="225" t="str">
+      <c r="AS18" s="225">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="AT18" s="227">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="AU18" s="226" t="str">
         <f>IFERROR((IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Movimentaçao | Mês Atual]])),((Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]])/Dados[[#This Row],[Saldo Bruto | Mês Anterior]]))-1)/(1-(IF(Dados[[#This Row],[Gross-Up]]="",0,Dados[[#This Row],[Gross-Up]]))),"0,00%")</f>
@@ -19275,7 +19330,7 @@
       </c>
       <c r="AV18" s="227">
         <f>IF(Dados[[#This Row],[Saldo Líquido | Mês Anterior]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido | Relatório]]=0,Dados[[#This Row],[Saldo Líquido | Relatório]],IF(Dados[[#This Row],[Saldo Líquido Esperado]]="",Dados[[#This Row],[Saldo Líquido | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Líquido Esperado]],Dados[[#This Row],[Saldo Líquido | Relatório]]))))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AW18" s="227">
         <f>IF(Dados[[#This Row],[Saldo Bruto | Mês Anterior]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto | Relatório]]=0,Dados[[#This Row],[Saldo Bruto | Relatório]],IF(Dados[[#This Row],[Saldo Bruto Esperado]]="",Dados[[#This Row],[Saldo Bruto | Relatório]],IF($AA$2=TRUE,Dados[[#This Row],[Saldo Bruto Esperado]],Dados[[#This Row],[Saldo Bruto | Relatório]]))))</f>
@@ -19299,17 +19354,17 @@
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
         <v>0</v>
       </c>
-      <c r="BD18" s="225" t="str">
+      <c r="BD18" s="225">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BE18" s="225">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF18" s="225" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF18" s="225">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BG18" s="225" cm="1">
         <f t="array" ref="BG18">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
@@ -19396,8 +19451,9 @@
         <f t="array" ref="Y19">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z19" s="55">
-        <v>30</v>
+      <c r="Z19" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA19" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
@@ -19427,9 +19483,9 @@
       <c r="AQ19" s="56">
         <v>0</v>
       </c>
-      <c r="AS19" s="51" t="str">
+      <c r="AS19" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="AT19" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
@@ -19464,21 +19520,21 @@
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
         <v>0</v>
       </c>
-      <c r="BD19" s="51" t="str">
+      <c r="BD19" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BE19" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF19" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF19" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BG19" s="51" cm="1">
         <f t="array" ref="BG19">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
+        <v>-0.96538747435533001</v>
       </c>
       <c r="BH19" s="51" t="str">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
@@ -19561,8 +19617,9 @@
         <f t="array" ref="Y20">IFERROR(_xlfn.IFS((Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="%"),(Dados[[#This Row],[Taxa]]*(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))),(Dados[[#This Row],[Subclasse]]="Pós-Fixado")*(Dados[[#This Row],[Pós-Fixado]]="+"),((((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[CDI]))))-1),(Dados[[#This Row],[Subclasse]]="Inflação"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))*(1+(_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[IPCA Cálculo])))-1),(Dados[[#This Row],[Subclasse]]="Prefixado"),(((1+Dados[[#This Row],[Taxa]])^((_xlfn.XLOOKUP($A$3,TabelaHistóricoDados[Mês],TabelaHistóricoDados[Dias Úteis])/252)))-1)),"")</f>
         <v/>
       </c>
-      <c r="Z20" s="55">
-        <v>30</v>
+      <c r="Z20" s="55" t="str">
+        <f>IFERROR((1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Líquido | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],"")</f>
+        <v/>
       </c>
       <c r="AA20" s="55" t="str">
         <f>IFERROR(IF(Dados[[#This Row],[Classe]]="Renda Fixa",(1+Dados[[#This Row],[Taxa | Esperada]])*Dados[[#This Row],[Saldo Bruto | Mês Anterior]]+Dados[[#This Row],[Juros / Dividendos]],""),"")</f>
@@ -19592,9 +19649,9 @@
       <c r="AQ20" s="56">
         <v>0</v>
       </c>
-      <c r="AS20" s="51" t="str">
+      <c r="AS20" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Bruto | Mês Atual]]/SUM(Dados[Saldo Bruto | Mês Atual]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="AT20" s="56">
         <f>Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Saldo Líquido | Mês Atual]]</f>
@@ -19629,21 +19686,21 @@
         <f>IF(Dados[[#This Row],[Participação]]="",IF(Dados[[#This Row],[Movimentaçao | Mês Atual]]&gt;0,Dados[[#This Row],[Saldo Bruto | Mês Atual]],Dados[[#This Row],[Saldo Bruto | Mês Atual]]-Dados[[#This Row],[Movimentaçao | Mês Atual]]),0)</f>
         <v>0</v>
       </c>
-      <c r="BD20" s="51" t="str">
+      <c r="BD20" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUM(Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BE20" s="51">
         <f>IFERROR(SUMPRODUCT(Dados[Performance | Mês Atual],Dados[Peso Corrigido | Carteira]),"0,00%")</f>
-        <v>0</v>
-      </c>
-      <c r="BF20" s="51" t="str">
+        <v>-0.78986247901799733</v>
+      </c>
+      <c r="BF20" s="51">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Custódia],Dados[[#This Row],[Custódia]],Dados[Saldo Corrigido]),"0,00%")</f>
-        <v>0,00%</v>
+        <v>0</v>
       </c>
       <c r="BG20" s="51" cm="1">
         <f t="array" ref="BG20">IFERROR(SUMPRODUCT((_xlfn._xlws.FILTER(Dados[Peso Corrigido | Custódia],Dados[Custódia]=Dados[[#This Row],[Custódia]])),_xlfn._xlws.FILTER(Dados[Performance | Mês Atual],Dados[Custódia]=Dados[[#This Row],[Custódia]])),"0,00%")</f>
-        <v>0</v>
+        <v>-0.96538747435533001</v>
       </c>
       <c r="BH20" s="51" t="str">
         <f>IFERROR(Dados[[#This Row],[Saldo Corrigido]]/SUMIF(Dados[Subclasse],Dados[[#This Row],[Subclasse]],Dados[Saldo Corrigido]),"0,00%")</f>
@@ -19896,7 +19953,7 @@
       <c r="U3" s="36"/>
       <c r="V3" s="39">
         <f>$H$11</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="W3" s="215">
         <f>$I$11</f>
@@ -19908,7 +19965,7 @@
       </c>
       <c r="Y3" s="40">
         <f>$K$11</f>
-        <v>0</v>
+        <v>8.7545454545454558E-3</v>
       </c>
       <c r="Z3" s="40">
         <f>$K$4</f>
@@ -20000,7 +20057,7 @@
       </c>
       <c r="H4" s="24">
         <f>IF(G4="","",SUMIF(Dados[Custódia],G4,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="I4" s="24">
         <f>IF(G4="","",SUMIF(Dados[Custódia],G4,Dados[Movimentaçao | Mês Atual]))</f>
@@ -20008,14 +20065,14 @@
       </c>
       <c r="J4" s="42">
         <f>IF(G4="","",SUMIF(Dados[Custódia],G4,Dados[Peso Corrigido | Carteira]))</f>
-        <v>0</v>
+        <v>0.81818181818181834</v>
       </c>
       <c r="K4" s="42">
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="L4" s="42">
         <f>IF(G4="","",_xlfn.XLOOKUP(G4,Dados[Custódia],Dados[Performance Custódia]))</f>
-        <v>0</v>
+        <v>-0.96538747435533001</v>
       </c>
       <c r="AI4" t="str" cm="1">
         <f t="array" ref="AI4:AI6">_xlfn._xlws.SORT(_xlfn.UNIQUE(Dados[Custódia]),1,1)</f>
@@ -20023,19 +20080,19 @@
       </c>
       <c r="AJ4" s="24">
         <f>IF(AI4="","",SUMIF(Dados[Custódia],AI4,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="AK4" s="24">
         <f>IF(AI4="","",SUMIF(Dados[Custódia],AI4,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AL4" s="26" t="e">
+      <c r="AL4" s="26">
         <f>IF(AI4="","",AJ4/SUM($AJ$4:$AJ$27))</f>
-        <v>#DIV/0!</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="AM4" s="26">
         <f>IF(AI4="","",_xlfn.XLOOKUP(AI4,Dados[Custódia],Dados[Performance Custódia]))</f>
-        <v>0</v>
+        <v>-0.96538747435533001</v>
       </c>
       <c r="AO4" t="str" cm="1">
         <f t="array" ref="AO4:AO8">_xlfn._xlws.SORT(_xlfn.UNIQUE(Dados[Subclasse]),1,1)</f>
@@ -20043,15 +20100,15 @@
       </c>
       <c r="AP4" s="24">
         <f>IF(AO4="","",SUMIF(Dados[Subclasse],AO4,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="AQ4" s="24">
         <f>IF(AO4="","",SUMIF(Dados[Movimentaçao | Mês Atual],AO4,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AR4" s="26" t="e">
+      <c r="AR4" s="26">
         <f>IF(AO4="","",AP4/SUM($AP$4:$AP$27))</f>
-        <v>#DIV/0!</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="AS4" s="26">
         <f>IF(AO4="","",_xlfn.XLOOKUP(AO4,Dados[Subclasse],Dados[Performance SubClasse]))</f>
@@ -20063,15 +20120,15 @@
       </c>
       <c r="AV4" s="24">
         <f>IF(AU4="","",SUMIF(Dados[Classe],AU4,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="AW4" s="24">
         <f>IF(AU4="","",SUMIF(Dados[Classe],AU4,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AX4" s="26" t="e">
+      <c r="AX4" s="26">
         <f>IF(AU4="","",AV4/SUM($AV$4:$AV$27))</f>
-        <v>#DIV/0!</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="AY4" s="26">
         <f>IF(AU4="","",_xlfn.XLOOKUP(AU4,Dados[Classe],Dados[Performance Classe]))</f>
@@ -20097,7 +20154,7 @@
       </c>
       <c r="H5" s="25">
         <f>IF(G5="","",SUMIF(Dados[Custódia],G5,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I5" s="25">
         <f>IF(G5="","",SUMIF(Dados[Custódia],G5,Dados[Movimentaçao | Mês Atual]))</f>
@@ -20105,7 +20162,7 @@
       </c>
       <c r="J5" s="43">
         <f>IF(G5="","",SUMIF(Dados[Custódia],G5,Dados[Peso Corrigido | Carteira]))</f>
-        <v>0</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="K5" s="43"/>
       <c r="L5" s="43">
@@ -20130,15 +20187,15 @@
       </c>
       <c r="AJ5" s="25">
         <f>IF(AI5="","",SUMIF(Dados[Custódia],AI5,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AK5" s="25">
         <f>IF(AI5="","",SUMIF(Dados[Custódia],AI5,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AL5" s="27" t="e">
+      <c r="AL5" s="27">
         <f t="shared" ref="AL5:AL27" si="0">IF(AI5="","",AJ5/SUM($AJ$4:$AJ$27))</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AM5" s="27">
         <f>IF(AI5="","",_xlfn.XLOOKUP(AI5,Dados[Custódia],Dados[Performance Custódia]))</f>
@@ -20149,38 +20206,38 @@
       </c>
       <c r="AP5" s="25">
         <f>IF(AO5="","",SUMIF(Dados[Subclasse],AO5,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AQ5" s="25">
         <f>IF(AO5="","",SUMIF(Dados[Movimentaçao | Mês Atual],AO5,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AR5" s="27" t="e">
+      <c r="AR5" s="27">
         <f t="shared" ref="AR5:AR27" si="1">IF(AO5="","",AP5/SUM($AP$4:$AP$27))</f>
-        <v>#DIV/0!</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="AS5" s="27">
         <f>IF(AO5="","",_xlfn.XLOOKUP(AO5,Dados[Subclasse],Dados[Performance SubClasse]))</f>
-        <v>0</v>
+        <v>-1.1736916893841964</v>
       </c>
       <c r="AU5" s="23" t="str">
         <v>Fundos de Investimento</v>
       </c>
       <c r="AV5" s="25">
         <f>IF(AU5="","",SUMIF(Dados[Classe],AU5,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AW5" s="25">
         <f>IF(AU5="","",SUMIF(Dados[Classe],AU5,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AX5" s="27" t="e">
+      <c r="AX5" s="27">
         <f t="shared" ref="AX5:AX27" si="2">IF(AU5="","",AV5/SUM($AV$4:$AV$27))</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AY5" s="27">
         <f>IF(AU5="","",_xlfn.XLOOKUP(AU5,Dados[Classe],Dados[Performance Classe]))</f>
-        <v>0</v>
+        <v>-0.99847249326980536</v>
       </c>
     </row>
     <row r="6" spans="2:51">
@@ -20202,7 +20259,7 @@
       </c>
       <c r="H6" s="24">
         <f>IF(G6="","",SUMIF(Dados[Custódia],G6,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I6" s="24">
         <f>IF(G6="","",SUMIF(Dados[Custódia],G6,Dados[Movimentaçao | Mês Atual]))</f>
@@ -20210,7 +20267,7 @@
       </c>
       <c r="J6" s="42">
         <f>IF(G6="","",SUMIF(Dados[Custódia],G6,Dados[Peso Corrigido | Carteira]))</f>
-        <v>0</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="K6" s="42"/>
       <c r="L6" s="42">
@@ -20279,15 +20336,15 @@
       </c>
       <c r="AJ6" s="24">
         <f>IF(AI6="","",SUMIF(Dados[Custódia],AI6,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AK6" s="24">
         <f>IF(AI6="","",SUMIF(Dados[Custódia],AI6,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AL6" s="26" t="e">
+      <c r="AL6" s="26">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AM6" s="26">
         <f>IF(AI6="","",_xlfn.XLOOKUP(AI6,Dados[Custódia],Dados[Performance Custódia]))</f>
@@ -20298,19 +20355,19 @@
       </c>
       <c r="AP6" s="24">
         <f>IF(AO6="","",SUMIF(Dados[Subclasse],AO6,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="AQ6" s="24">
         <f>IF(AO6="","",SUMIF(Dados[Movimentaçao | Mês Atual],AO6,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AR6" s="26" t="e">
+      <c r="AR6" s="26">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="AS6" s="26">
         <f>IF(AO6="","",_xlfn.XLOOKUP(AO6,Dados[Subclasse],Dados[Performance SubClasse]))</f>
-        <v>0</v>
+        <v>-1.0685262794319546</v>
       </c>
       <c r="AU6" t="str">
         <v>Previdência</v>
@@ -20323,9 +20380,9 @@
         <f>IF(AU6="","",SUMIF(Dados[Classe],AU6,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AX6" s="26" t="e">
+      <c r="AX6" s="26">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AY6" s="26">
         <f>IF(AU6="","",_xlfn.XLOOKUP(AU6,Dados[Classe],Dados[Performance Classe]))</f>
@@ -20450,9 +20507,9 @@
         <f>IF(AO7="","",SUMIF(Dados[Movimentaçao | Mês Atual],AO7,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AR7" s="27" t="e">
+      <c r="AR7" s="27">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AS7" s="27">
         <f>IF(AO7="","",_xlfn.XLOOKUP(AO7,Dados[Subclasse],Dados[Performance SubClasse]))</f>
@@ -20463,19 +20520,19 @@
       </c>
       <c r="AV7" s="25">
         <f>IF(AU7="","",SUMIF(Dados[Classe],AU7,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="AW7" s="25">
         <f>IF(AU7="","",SUMIF(Dados[Classe],AU7,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AX7" s="27" t="e">
+      <c r="AX7" s="27">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="AY7" s="27">
         <f>IF(AU7="","",_xlfn.XLOOKUP(AU7,Dados[Classe],Dados[Performance Classe]))</f>
-        <v>0</v>
+        <v>-1.0985735394183094</v>
       </c>
     </row>
     <row r="8" spans="2:51">
@@ -20588,19 +20645,19 @@
       </c>
       <c r="AP8" s="24">
         <f>IF(AO8="","",SUMIF(Dados[Subclasse],AO8,Dados[Saldo Bruto | Mês Atual]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AQ8" s="24">
         <f>IF(AO8="","",SUMIF(Dados[Movimentaçao | Mês Atual],AO8,Dados[Movimentaçao | Mês Atual]))</f>
         <v>0</v>
       </c>
-      <c r="AR8" s="26" t="e">
+      <c r="AR8" s="26">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AS8" s="26">
         <f>IF(AO8="","",_xlfn.XLOOKUP(AO8,Dados[Subclasse],Dados[Performance SubClasse]))</f>
-        <v>0</v>
+        <v>-0.99847249326980536</v>
       </c>
       <c r="AV8" s="24" t="str">
         <f>IF(AU8="","",SUMIF(Dados[Classe],AU8,Dados[Saldo Bruto | Mês Atual]))</f>
@@ -20904,7 +20961,7 @@
       </c>
       <c r="H11" s="34">
         <f>SUM(H4:H9)</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="I11" s="34">
         <f>SUM(I4:I9)</f>
@@ -20912,15 +20969,15 @@
       </c>
       <c r="J11" s="21">
         <f>SUM(J4:J9)</f>
-        <v>0</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="K11" s="165">
         <f>SUMPRODUCT($J$4:$J$9,$K$4:$K$9)</f>
-        <v>0</v>
+        <v>8.7545454545454558E-3</v>
       </c>
       <c r="L11" s="35">
         <f>SUMPRODUCT($J$4:$J$9,$L$4:$L$9)</f>
-        <v>0</v>
+        <v>-0.78986247901799744</v>
       </c>
       <c r="N11" s="41">
         <v>45323</v>
@@ -21044,7 +21101,7 @@
       </c>
       <c r="E12">
         <f>COUNTIFS(Dados[Subclasse],ClasseSubClasse[[#This Row],[SubClasse]],Dados[Lista?],TRUE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N12" s="41">
         <v>45292</v>
@@ -25099,23 +25156,23 @@
       </c>
       <c r="R3" s="127" cm="1">
         <f t="array" ref="R3:R17">Dados[Saldo Bruto | Mês Atual]</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S3" s="127" cm="1">
         <f t="array" ref="S3:S17">Dados[Movimentaçao | Mês Atual]</f>
         <v>0</v>
       </c>
-      <c r="T3" s="31" t="str" cm="1">
+      <c r="T3" s="31" cm="1">
         <f t="array" ref="T3:T17">Dados[Peso | Mês Atual]</f>
-        <v>0,00%</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="U3" s="31" cm="1">
         <f t="array" ref="U3:U17">Dados[Performance | Mês Atual]</f>
-        <v>-1</v>
+        <v>-0.99847249326980536</v>
       </c>
       <c r="V3" s="29" cm="1">
         <f t="array" ref="V3:V17">Dados[Saldo Corrigido]</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -25174,19 +25231,19 @@
         <v>Renda Fixa - Prefixado</v>
       </c>
       <c r="R4" s="127">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="S4" s="127">
         <v>0</v>
       </c>
-      <c r="T4" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T4" s="31">
+        <v>0.18181818181818182</v>
       </c>
       <c r="U4" s="31">
-        <v>-1</v>
+        <v>-0.99840691830772665</v>
       </c>
       <c r="V4" s="29">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -25245,19 +25302,19 @@
         <v>Renda Fixa - Prefixado</v>
       </c>
       <c r="R5" s="127">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S5" s="127">
         <v>0</v>
       </c>
-      <c r="T5" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T5" s="31">
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="U5" s="31">
-        <v>-1</v>
+        <v>-0.9984028202361398</v>
       </c>
       <c r="V5" s="29">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -25316,19 +25373,19 @@
         <v>Conta Corrente</v>
       </c>
       <c r="R6" s="127">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S6" s="127">
         <v>0</v>
       </c>
-      <c r="T6" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T6" s="31">
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="U6" s="31" t="str">
         <v>0,00%</v>
       </c>
       <c r="V6" s="29">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -25387,19 +25444,19 @@
         <v>Conta Corrente</v>
       </c>
       <c r="R7" s="127">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S7" s="127">
         <v>0</v>
       </c>
-      <c r="T7" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T7" s="31">
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="U7" s="31" t="str">
         <v>0,00%</v>
       </c>
       <c r="V7" s="29">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -25458,19 +25515,19 @@
         <v>Conta Corrente</v>
       </c>
       <c r="R8" s="127">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S8" s="127">
         <v>0</v>
       </c>
-      <c r="T8" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T8" s="31">
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="U8" s="31" t="str">
         <v>0,00%</v>
       </c>
       <c r="V8" s="29">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -25529,19 +25586,19 @@
         <v>Renda Fixa - Prefixado</v>
       </c>
       <c r="R9" s="127">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S9" s="127">
         <v>0</v>
       </c>
-      <c r="T9" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T9" s="31">
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="U9" s="31">
-        <v>-1.1764705882352942</v>
+        <v>-1.1754564963690872</v>
       </c>
       <c r="V9" s="29">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -25600,19 +25657,19 @@
         <v>Renda Fixa - Inflação</v>
       </c>
       <c r="R10" s="127">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S10" s="127">
         <v>0</v>
       </c>
-      <c r="T10" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T10" s="31">
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="U10" s="31">
-        <v>-1.1764705882352942</v>
+        <v>-1.1754039076648017</v>
       </c>
       <c r="V10" s="29">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -25671,19 +25728,19 @@
         <v>Renda Fixa - Prefixado</v>
       </c>
       <c r="R11" s="127">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S11" s="127">
         <v>0</v>
       </c>
-      <c r="T11" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T11" s="31">
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="U11" s="31">
-        <v>-1.1764705882352942</v>
+        <v>-1.1719582439390925</v>
       </c>
       <c r="V11" s="29">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -25742,19 +25799,19 @@
         <v>Renda Fixa - Inflação</v>
       </c>
       <c r="R12" s="127">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S12" s="127">
         <v>0</v>
       </c>
-      <c r="T12" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T12" s="31">
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="U12" s="31">
-        <v>-1.1764705882352942</v>
+        <v>-1.1719794711035911</v>
       </c>
       <c r="V12" s="29">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -25818,8 +25875,8 @@
       <c r="S13" s="127">
         <v>0</v>
       </c>
-      <c r="T13" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T13" s="31">
+        <v>0</v>
       </c>
       <c r="U13" s="31">
         <v>-1.1764705882352942</v>
@@ -25889,8 +25946,8 @@
       <c r="S14" s="127">
         <v>0</v>
       </c>
-      <c r="T14" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T14" s="31">
+        <v>0</v>
       </c>
       <c r="U14" s="31" t="str">
         <v>0,00%</v>
@@ -25960,8 +26017,8 @@
       <c r="S15" s="127">
         <v>0</v>
       </c>
-      <c r="T15" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T15" s="31">
+        <v>0</v>
       </c>
       <c r="U15" s="31" t="str">
         <v>0,00%</v>
@@ -26031,8 +26088,8 @@
       <c r="S16" s="127">
         <v>0</v>
       </c>
-      <c r="T16" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T16" s="31">
+        <v>0</v>
       </c>
       <c r="U16" s="31">
         <v>-1</v>
@@ -26102,8 +26159,8 @@
       <c r="S17" s="127">
         <v>0</v>
       </c>
-      <c r="T17" s="31" t="str">
-        <v>0,00%</v>
+      <c r="T17" s="31">
+        <v>0</v>
       </c>
       <c r="U17" s="31">
         <v>-1</v>

</xml_diff>